<commit_message>
burndown rapp and project
</commit_message>
<xml_diff>
--- a/Burndown_chart ensas(1).xlsx
+++ b/Burndown_chart ensas(1).xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rakhi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp12\htdocs\Nouveau dossier\GL_PROJECT\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5BFA66-093F-41FF-813A-DB73FEB3CD8A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -122,7 +123,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -211,6 +212,7 @@
         <sz val="12"/>
         <color rgb="FF24292E"/>
         <name val="Segoe UI"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -228,6 +230,7 @@
         <sz val="12"/>
         <color rgb="FF24292E"/>
         <name val="Segoe UI"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -245,6 +248,7 @@
         <sz val="12"/>
         <color rgb="FF24292E"/>
         <name val="Segoe UI"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -262,6 +266,7 @@
         <sz val="12"/>
         <color rgb="FF24292E"/>
         <name val="Segoe UI"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -279,6 +284,7 @@
         <sz val="12"/>
         <color rgb="FF24292E"/>
         <name val="Segoe UI"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -296,6 +302,7 @@
         <sz val="12"/>
         <color rgb="FF24292E"/>
         <name val="Segoe UI"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -316,6 +323,7 @@
         <sz val="12"/>
         <color rgb="FF24292E"/>
         <name val="Segoe UI"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -461,9 +469,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -632,9 +640,8 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -693,13 +700,13 @@
                   <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>11</c:v>
@@ -708,7 +715,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-9AE3-4045-8805-051F8DEDD032}"/>
             </c:ext>
@@ -780,9 +787,8 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -856,7 +862,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-9AE3-4045-8805-051F8DEDD032}"/>
             </c:ext>
@@ -921,7 +927,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1049,7 +1054,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1812,7 +1816,7 @@
         <xdr:cNvPr id="7" name="TextBox 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1875,7 +1879,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1897,17 +1901,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B6:I22" totalsRowCount="1">
-  <autoFilter ref="B6:I21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B6:I22" totalsRowCount="1">
+  <autoFilter ref="B6:I21" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Feature" totalsRowLabel="Burndown" dataDxfId="15" totalsRowDxfId="7"/>
-    <tableColumn id="3" name="Estimated Hours" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="6"/>
-    <tableColumn id="4" name="Status" dataDxfId="13" totalsRowDxfId="5"/>
-    <tableColumn id="5" name="Day 1" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="4"/>
-    <tableColumn id="6" name="Day 2" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="3"/>
-    <tableColumn id="9" name="Day 3" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="2"/>
-    <tableColumn id="7" name="Day 4" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="1"/>
-    <tableColumn id="8" name="Day 5" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Feature" totalsRowLabel="Burndown" dataDxfId="15" totalsRowDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Estimated Hours" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Status" dataDxfId="13" totalsRowDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Day 1" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Day 2" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Day 3" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Day 4" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Day 5" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2209,23 +2213,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="AC28" sqref="AC28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.453125" customWidth="1"/>
-    <col min="2" max="2" width="137.81640625" customWidth="1"/>
-    <col min="3" max="3" width="18.08984375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15.453125" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="2" max="2" width="137.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="21.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2251,7 +2255,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
@@ -2267,22 +2271,22 @@
       </c>
       <c r="F3" s="1">
         <f>IF(SUM(Table1[[Day 2]:[Day 5]])=0,#N/A,$D3-SUM(Table1[[Day 1]:[Day 2]]))</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G3" s="1">
         <f>IF(SUM(Table1[[Day 3]:[Day 5]])=0,#N/A,$D3-SUM(Table1[[Day 1]:[Day 3]]))</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H3" s="1">
         <f>IF(SUM(Table1[[Day 4]:[Day 5]])=0,#N/A,$D3-SUM(Table1[[Day 1]:[Day 4]]))</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I3" s="1">
         <f>IF(SUM(Table1[[Day 5]:[Day 5]])=0,#N/A,$D3-SUM(Table1[[Day 1]:[Day 5]]))</f>
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -2313,7 +2317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
@@ -2339,7 +2343,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
@@ -2365,7 +2369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>16</v>
       </c>
@@ -2391,7 +2395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
@@ -2417,7 +2421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>18</v>
       </c>
@@ -2443,7 +2447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>19</v>
       </c>
@@ -2469,7 +2473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>20</v>
       </c>
@@ -2495,7 +2499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>21</v>
       </c>
@@ -2521,7 +2525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>22</v>
       </c>
@@ -2547,7 +2551,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>23</v>
       </c>
@@ -2573,7 +2577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
         <v>24</v>
       </c>
@@ -2587,7 +2591,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G16" s="3">
         <v>0</v>
@@ -2596,10 +2600,10 @@
         <v>0</v>
       </c>
       <c r="I16" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>25</v>
       </c>
@@ -2625,7 +2629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>26</v>
       </c>
@@ -2651,7 +2655,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
         <v>27</v>
       </c>
@@ -2677,7 +2681,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
         <v>28</v>
       </c>
@@ -2703,7 +2707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
         <v>29</v>
       </c>
@@ -2729,7 +2733,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>30</v>
       </c>
@@ -2744,7 +2748,7 @@
       </c>
       <c r="F22" s="3">
         <f>SUBTOTAL(109,Table1[Day 2])</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G22" s="3">
         <f>SUBTOTAL(109,Table1[Day 3])</f>
@@ -2756,7 +2760,7 @@
       </c>
       <c r="I22" s="3">
         <f>SUBTOTAL(109,Table1[Day 5])</f>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>